<commit_message>
Add borders for Libro Mayor
</commit_message>
<xml_diff>
--- a/Excel/Contabilidad.xlsx
+++ b/Excel/Contabilidad.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6366" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10926" uniqueCount="466">
   <si>
     <t>Libro Diario</t>
   </si>
@@ -1439,7 +1439,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1468,11 +1468,84 @@
         <color rgb="FFAAAAAA"/>
       </bottom>
     </border>
+    <border>
+      <top style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <top style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="205">
+  <cellXfs count="366">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -1946,6 +2019,449 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4019,7 +4535,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="158">
+      <c r="A1" t="s" s="311">
         <v>181</v>
       </c>
     </row>
@@ -4977,22 +5493,29 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="159">
+      <c r="A1" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B1" s="312"/>
+      <c r="C1" s="312"/>
+      <c r="D1" s="312"/>
+      <c r="E1" s="312"/>
+      <c r="F1" s="318"/>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="314">
         <v>263</v>
       </c>
+      <c r="F2" s="315"/>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="314">
         <v>264</v>
       </c>
+      <c r="F3" s="315"/>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B4" t="s">
@@ -5007,12 +5530,12 @@
       <c r="E4" t="s">
         <v>269</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="314">
         <v>5</v>
       </c>
       <c r="B5" t="s">
@@ -5027,12 +5550,12 @@
       <c r="E5" t="s">
         <v>193</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="315">
         <v>216</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="314">
         <v>64</v>
       </c>
       <c r="B6" t="s">
@@ -5047,12 +5570,12 @@
       <c r="E6" t="s">
         <v>214</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="315">
         <v>271</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="314">
         <v>64</v>
       </c>
       <c r="B7" t="s">
@@ -5067,12 +5590,12 @@
       <c r="E7" t="s">
         <v>193</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" t="s" s="315">
         <v>273</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="314">
         <v>64</v>
       </c>
       <c r="B8" t="s">
@@ -5087,12 +5610,12 @@
       <c r="E8" t="s">
         <v>272</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" t="s" s="315">
         <v>271</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="314">
         <v>101</v>
       </c>
       <c r="B9" t="s">
@@ -5107,12 +5630,12 @@
       <c r="E9" t="s">
         <v>194</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" t="s" s="315">
         <v>274</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="314">
         <v>107</v>
       </c>
       <c r="B10" t="s">
@@ -5127,12 +5650,12 @@
       <c r="E10" t="s">
         <v>193</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" t="s" s="315">
         <v>276</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="314">
         <v>113</v>
       </c>
       <c r="B11" t="s">
@@ -5147,12 +5670,12 @@
       <c r="E11" t="s">
         <v>193</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" t="s" s="315">
         <v>278</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="314">
         <v>127</v>
       </c>
       <c r="B12" t="s">
@@ -5167,47 +5690,54 @@
       <c r="E12" t="s">
         <v>279</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" t="s" s="315">
         <v>192</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" t="s" s="313">
         <v>190</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="s" s="313">
         <v>191</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" t="s" s="316">
         <v>192</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="160">
+      <c r="A17" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B17" s="312"/>
+      <c r="C17" s="312"/>
+      <c r="D17" s="312"/>
+      <c r="E17" s="312"/>
+      <c r="F17" s="318"/>
     </row>
     <row r="18">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="314">
         <v>282</v>
       </c>
+      <c r="F18" s="315"/>
     </row>
     <row r="19">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="314">
         <v>283</v>
       </c>
+      <c r="F19" s="315"/>
     </row>
     <row r="20">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B20" t="s">
@@ -5222,12 +5752,12 @@
       <c r="E20" t="s">
         <v>269</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="314">
         <v>89</v>
       </c>
       <c r="B21" t="s">
@@ -5242,12 +5772,12 @@
       <c r="E21" t="s">
         <v>193</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" t="s" s="315">
         <v>194</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="314">
         <v>146</v>
       </c>
       <c r="B22" t="s">
@@ -5262,47 +5792,54 @@
       <c r="E22" t="s">
         <v>195</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" t="s" s="315">
         <v>196</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" t="s" s="313">
         <v>194</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="s" s="313">
         <v>195</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" t="s" s="316">
         <v>196</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s" s="161">
+      <c r="A27" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B27" s="312"/>
+      <c r="C27" s="312"/>
+      <c r="D27" s="312"/>
+      <c r="E27" s="312"/>
+      <c r="F27" s="318"/>
     </row>
     <row r="28">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="314">
         <v>284</v>
       </c>
+      <c r="F28" s="315"/>
     </row>
     <row r="29">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="314">
         <v>285</v>
       </c>
+      <c r="F29" s="315"/>
     </row>
     <row r="30">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B30" t="s">
@@ -5317,12 +5854,12 @@
       <c r="E30" t="s">
         <v>269</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="314">
         <v>64</v>
       </c>
       <c r="B31" t="s">
@@ -5337,12 +5874,12 @@
       <c r="E31" t="s">
         <v>193</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" t="s" s="315">
         <v>214</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="314">
         <v>64</v>
       </c>
       <c r="B32" t="s">
@@ -5357,12 +5894,12 @@
       <c r="E32" t="s">
         <v>193</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" t="s" s="315">
         <v>286</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="314">
         <v>89</v>
       </c>
       <c r="B33" t="s">
@@ -5377,12 +5914,12 @@
       <c r="E33" t="s">
         <v>212</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" t="s" s="315">
         <v>273</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
+      <c r="A34" t="s" s="314">
         <v>89</v>
       </c>
       <c r="B34" t="s">
@@ -5397,12 +5934,12 @@
       <c r="E34" t="s">
         <v>287</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" t="s" s="315">
         <v>288</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
+      <c r="A35" t="s" s="314">
         <v>89</v>
       </c>
       <c r="B35" t="s">
@@ -5417,12 +5954,12 @@
       <c r="E35" t="s">
         <v>194</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" t="s" s="315">
         <v>289</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
+      <c r="A36" t="s" s="314">
         <v>97</v>
       </c>
       <c r="B36" t="s">
@@ -5437,12 +5974,12 @@
       <c r="E36" t="s">
         <v>290</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" t="s" s="315">
         <v>291</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
+      <c r="A37" t="s" s="314">
         <v>127</v>
       </c>
       <c r="B37" t="s">
@@ -5457,12 +5994,12 @@
       <c r="E37" t="s">
         <v>210</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" t="s" s="315">
         <v>292</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
+      <c r="A38" t="s" s="314">
         <v>127</v>
       </c>
       <c r="B38" t="s">
@@ -5477,12 +6014,12 @@
       <c r="E38" t="s">
         <v>249</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" t="s" s="315">
         <v>293</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
+      <c r="A39" t="s" s="314">
         <v>146</v>
       </c>
       <c r="B39" t="s">
@@ -5497,12 +6034,12 @@
       <c r="E39" t="s">
         <v>210</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" t="s" s="315">
         <v>294</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
+      <c r="A40" t="s" s="314">
         <v>158</v>
       </c>
       <c r="B40" t="s">
@@ -5517,12 +6054,12 @@
       <c r="E40" t="s">
         <v>210</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" t="s" s="315">
         <v>295</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s">
+      <c r="A41" t="s" s="314">
         <v>161</v>
       </c>
       <c r="B41" t="s">
@@ -5537,12 +6074,12 @@
       <c r="E41" t="s">
         <v>193</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" t="s" s="315">
         <v>297</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
+      <c r="A42" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B42" t="s">
@@ -5557,12 +6094,12 @@
       <c r="E42" t="s">
         <v>193</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" t="s" s="315">
         <v>299</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s">
+      <c r="A43" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B43" t="s">
@@ -5577,47 +6114,54 @@
       <c r="E43" t="s">
         <v>300</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" t="s" s="315">
         <v>199</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
+      <c r="A44" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" t="s" s="313">
         <v>197</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" t="s" s="313">
         <v>198</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" t="s" s="316">
         <v>199</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s" s="162">
+      <c r="A48" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B48" s="312"/>
+      <c r="C48" s="312"/>
+      <c r="D48" s="312"/>
+      <c r="E48" s="312"/>
+      <c r="F48" s="318"/>
     </row>
     <row r="49">
-      <c r="A49" t="s">
+      <c r="A49" t="s" s="314">
         <v>301</v>
       </c>
+      <c r="F49" s="315"/>
     </row>
     <row r="50">
-      <c r="A50" t="s">
+      <c r="A50" t="s" s="314">
         <v>302</v>
       </c>
+      <c r="F50" s="315"/>
     </row>
     <row r="51">
-      <c r="A51" t="s">
+      <c r="A51" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B51" t="s">
@@ -5632,12 +6176,12 @@
       <c r="E51" t="s">
         <v>269</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s">
+      <c r="A52" t="s" s="314">
         <v>5</v>
       </c>
       <c r="B52" t="s">
@@ -5652,12 +6196,12 @@
       <c r="E52" t="s">
         <v>193</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" t="s" s="315">
         <v>303</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="s">
+      <c r="A53" t="s" s="314">
         <v>113</v>
       </c>
       <c r="B53" t="s">
@@ -5672,12 +6216,12 @@
       <c r="E53" t="s">
         <v>193</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" t="s" s="315">
         <v>200</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="s">
+      <c r="A54" t="s" s="314">
         <v>127</v>
       </c>
       <c r="B54" t="s">
@@ -5692,47 +6236,54 @@
       <c r="E54" t="s">
         <v>201</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" t="s" s="315">
         <v>202</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="s">
+      <c r="A55" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" t="s" s="313">
         <v>200</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" t="s" s="313">
         <v>201</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" t="s" s="316">
         <v>202</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s" s="163">
+      <c r="A59" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B59" s="312"/>
+      <c r="C59" s="312"/>
+      <c r="D59" s="312"/>
+      <c r="E59" s="312"/>
+      <c r="F59" s="318"/>
     </row>
     <row r="60">
-      <c r="A60" t="s">
+      <c r="A60" t="s" s="314">
         <v>305</v>
       </c>
+      <c r="F60" s="315"/>
     </row>
     <row r="61">
-      <c r="A61" t="s">
+      <c r="A61" t="s" s="314">
         <v>306</v>
       </c>
+      <c r="F61" s="315"/>
     </row>
     <row r="62">
-      <c r="A62" t="s">
+      <c r="A62" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B62" t="s">
@@ -5747,12 +6298,12 @@
       <c r="E62" t="s">
         <v>269</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="s">
+      <c r="A63" t="s" s="314">
         <v>89</v>
       </c>
       <c r="B63" t="s">
@@ -5767,12 +6318,12 @@
       <c r="E63" t="s">
         <v>193</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" t="s" s="315">
         <v>307</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="s">
+      <c r="A64" t="s" s="314">
         <v>97</v>
       </c>
       <c r="B64" t="s">
@@ -5787,12 +6338,12 @@
       <c r="E64" t="s">
         <v>193</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" t="s" s="315">
         <v>309</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s">
+      <c r="A65" t="s" s="314">
         <v>107</v>
       </c>
       <c r="B65" t="s">
@@ -5807,12 +6358,12 @@
       <c r="E65" t="s">
         <v>310</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" t="s" s="315">
         <v>311</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s">
+      <c r="A66" t="s" s="314">
         <v>146</v>
       </c>
       <c r="B66" t="s">
@@ -5827,12 +6378,12 @@
       <c r="E66" t="s">
         <v>193</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" t="s" s="315">
         <v>313</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="s">
+      <c r="A67" t="s" s="314">
         <v>153</v>
       </c>
       <c r="B67" t="s">
@@ -5847,12 +6398,12 @@
       <c r="E67" t="s">
         <v>193</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" t="s" s="315">
         <v>315</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="s">
+      <c r="A68" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B68" t="s">
@@ -5867,47 +6418,54 @@
       <c r="E68" t="s">
         <v>315</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="s">
+      <c r="A69" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" t="s" s="313">
         <v>203</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" t="s" s="313">
         <v>203</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="s" s="164">
+      <c r="A73" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B73" s="312"/>
+      <c r="C73" s="312"/>
+      <c r="D73" s="312"/>
+      <c r="E73" s="312"/>
+      <c r="F73" s="318"/>
     </row>
     <row r="74">
-      <c r="A74" t="s">
+      <c r="A74" t="s" s="314">
         <v>316</v>
       </c>
+      <c r="F74" s="315"/>
     </row>
     <row r="75">
-      <c r="A75" t="s">
+      <c r="A75" t="s" s="314">
         <v>317</v>
       </c>
+      <c r="F75" s="315"/>
     </row>
     <row r="76">
-      <c r="A76" t="s">
+      <c r="A76" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B76" t="s">
@@ -5922,12 +6480,12 @@
       <c r="E76" t="s">
         <v>269</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="s">
+      <c r="A77" t="s" s="314">
         <v>146</v>
       </c>
       <c r="B77" t="s">
@@ -5942,47 +6500,54 @@
       <c r="E77" t="s">
         <v>193</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" t="s" s="315">
         <v>204</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="s">
+      <c r="A78" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" t="s" s="313">
         <v>204</v>
       </c>
-      <c r="E78" t="s">
-        <v>193</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="E78" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="F78" t="s" s="316">
         <v>204</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="s" s="165">
+      <c r="A82" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B82" s="312"/>
+      <c r="C82" s="312"/>
+      <c r="D82" s="312"/>
+      <c r="E82" s="312"/>
+      <c r="F82" s="318"/>
     </row>
     <row r="83">
-      <c r="A83" t="s">
+      <c r="A83" t="s" s="314">
         <v>318</v>
       </c>
+      <c r="F83" s="315"/>
     </row>
     <row r="84">
-      <c r="A84" t="s">
+      <c r="A84" t="s" s="314">
         <v>319</v>
       </c>
+      <c r="F84" s="315"/>
     </row>
     <row r="85">
-      <c r="A85" t="s">
+      <c r="A85" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B85" t="s">
@@ -5997,12 +6562,12 @@
       <c r="E85" t="s">
         <v>269</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="s">
+      <c r="A86" t="s" s="314">
         <v>5</v>
       </c>
       <c r="B86" t="s">
@@ -6017,12 +6582,12 @@
       <c r="E86" t="s">
         <v>193</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" t="s" s="315">
         <v>320</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="s">
+      <c r="A87" t="s" s="314">
         <v>64</v>
       </c>
       <c r="B87" t="s">
@@ -6037,12 +6602,12 @@
       <c r="E87" t="s">
         <v>321</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" t="s" s="315">
         <v>322</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="s">
+      <c r="A88" t="s" s="314">
         <v>97</v>
       </c>
       <c r="B88" t="s">
@@ -6057,12 +6622,12 @@
       <c r="E88" t="s">
         <v>193</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" t="s" s="315">
         <v>324</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="s">
+      <c r="A89" t="s" s="314">
         <v>107</v>
       </c>
       <c r="B89" t="s">
@@ -6077,12 +6642,12 @@
       <c r="E89" t="s">
         <v>325</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" t="s" s="315">
         <v>326</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="s">
+      <c r="A90" t="s" s="314">
         <v>113</v>
       </c>
       <c r="B90" t="s">
@@ -6097,12 +6662,12 @@
       <c r="E90" t="s">
         <v>327</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" t="s" s="315">
         <v>328</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="s">
+      <c r="A91" t="s" s="314">
         <v>127</v>
       </c>
       <c r="B91" t="s">
@@ -6117,12 +6682,12 @@
       <c r="E91" t="s">
         <v>193</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F91" t="s" s="315">
         <v>329</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="s">
+      <c r="A92" t="s" s="314">
         <v>153</v>
       </c>
       <c r="B92" t="s">
@@ -6137,12 +6702,12 @@
       <c r="E92" t="s">
         <v>193</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F92" t="s" s="315">
         <v>331</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="s">
+      <c r="A93" t="s" s="314">
         <v>161</v>
       </c>
       <c r="B93" t="s">
@@ -6157,47 +6722,54 @@
       <c r="E93" t="s">
         <v>332</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" t="s" s="315">
         <v>208</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="s">
+      <c r="A94" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C94" t="n">
+      <c r="C94" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" t="s" s="313">
         <v>206</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" t="s" s="313">
         <v>207</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" t="s" s="316">
         <v>208</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="s" s="166">
+      <c r="A98" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B98" s="312"/>
+      <c r="C98" s="312"/>
+      <c r="D98" s="312"/>
+      <c r="E98" s="312"/>
+      <c r="F98" s="318"/>
     </row>
     <row r="99">
-      <c r="A99" t="s">
+      <c r="A99" t="s" s="314">
         <v>333</v>
       </c>
+      <c r="F99" s="315"/>
     </row>
     <row r="100">
-      <c r="A100" t="s">
+      <c r="A100" t="s" s="314">
         <v>334</v>
       </c>
+      <c r="F100" s="315"/>
     </row>
     <row r="101">
-      <c r="A101" t="s">
+      <c r="A101" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B101" t="s">
@@ -6212,12 +6784,12 @@
       <c r="E101" t="s">
         <v>269</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F101" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="s">
+      <c r="A102" t="s" s="314">
         <v>146</v>
       </c>
       <c r="B102" t="s">
@@ -6232,12 +6804,12 @@
       <c r="E102" t="s">
         <v>193</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" t="s" s="315">
         <v>210</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="s">
+      <c r="A103" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B103" t="s">
@@ -6252,47 +6824,54 @@
       <c r="E103" t="s">
         <v>210</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F103" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="s">
+      <c r="A104" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C104" t="n">
+      <c r="C104" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" t="s" s="313">
         <v>210</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" t="s" s="313">
         <v>210</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F104" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="s" s="167">
+      <c r="A108" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B108" s="312"/>
+      <c r="C108" s="312"/>
+      <c r="D108" s="312"/>
+      <c r="E108" s="312"/>
+      <c r="F108" s="318"/>
     </row>
     <row r="109">
-      <c r="A109" t="s">
+      <c r="A109" t="s" s="314">
         <v>335</v>
       </c>
+      <c r="F109" s="315"/>
     </row>
     <row r="110">
-      <c r="A110" t="s">
+      <c r="A110" t="s" s="314">
         <v>336</v>
       </c>
+      <c r="F110" s="315"/>
     </row>
     <row r="111">
-      <c r="A111" t="s">
+      <c r="A111" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B111" t="s">
@@ -6307,12 +6886,12 @@
       <c r="E111" t="s">
         <v>269</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F111" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="s">
+      <c r="A112" t="s" s="314">
         <v>89</v>
       </c>
       <c r="B112" t="s">
@@ -6327,47 +6906,54 @@
       <c r="E112" t="s">
         <v>193</v>
       </c>
-      <c r="F112" t="s">
+      <c r="F112" t="s" s="315">
         <v>212</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="s">
+      <c r="A113" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C113" t="n">
+      <c r="C113" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" t="s" s="313">
         <v>212</v>
       </c>
-      <c r="E113" t="s">
-        <v>193</v>
-      </c>
-      <c r="F113" t="s">
+      <c r="E113" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="F113" t="s" s="316">
         <v>212</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="s" s="168">
+      <c r="A117" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B117" s="312"/>
+      <c r="C117" s="312"/>
+      <c r="D117" s="312"/>
+      <c r="E117" s="312"/>
+      <c r="F117" s="318"/>
     </row>
     <row r="118">
-      <c r="A118" t="s">
+      <c r="A118" t="s" s="314">
         <v>337</v>
       </c>
+      <c r="F118" s="315"/>
     </row>
     <row r="119">
-      <c r="A119" t="s">
+      <c r="A119" t="s" s="314">
         <v>338</v>
       </c>
+      <c r="F119" s="315"/>
     </row>
     <row r="120">
-      <c r="A120" t="s">
+      <c r="A120" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B120" t="s">
@@ -6382,12 +6968,12 @@
       <c r="E120" t="s">
         <v>269</v>
       </c>
-      <c r="F120" t="s">
+      <c r="F120" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="s">
+      <c r="A121" t="s" s="314">
         <v>5</v>
       </c>
       <c r="B121" t="s">
@@ -6402,47 +6988,54 @@
       <c r="E121" t="s">
         <v>193</v>
       </c>
-      <c r="F121" t="s">
+      <c r="F121" t="s" s="315">
         <v>214</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="s">
+      <c r="A122" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C122" t="n">
+      <c r="C122" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" t="s" s="313">
         <v>214</v>
       </c>
-      <c r="E122" t="s">
-        <v>193</v>
-      </c>
-      <c r="F122" t="s">
+      <c r="E122" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="F122" t="s" s="316">
         <v>214</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="s" s="169">
+      <c r="A126" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B126" s="312"/>
+      <c r="C126" s="312"/>
+      <c r="D126" s="312"/>
+      <c r="E126" s="312"/>
+      <c r="F126" s="318"/>
     </row>
     <row r="127">
-      <c r="A127" t="s">
+      <c r="A127" t="s" s="314">
         <v>339</v>
       </c>
+      <c r="F127" s="315"/>
     </row>
     <row r="128">
-      <c r="A128" t="s">
+      <c r="A128" t="s" s="314">
         <v>340</v>
       </c>
+      <c r="F128" s="315"/>
     </row>
     <row r="129">
-      <c r="A129" t="s">
+      <c r="A129" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B129" t="s">
@@ -6457,12 +7050,12 @@
       <c r="E129" t="s">
         <v>269</v>
       </c>
-      <c r="F129" t="s">
+      <c r="F129" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="s">
+      <c r="A130" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B130" t="s">
@@ -6477,47 +7070,54 @@
       <c r="E130" t="s">
         <v>215</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F130" t="s" s="315">
         <v>341</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="s">
+      <c r="A131" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C131" t="n">
+      <c r="C131" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D131" t="s">
-        <v>193</v>
-      </c>
-      <c r="E131" t="s">
+      <c r="D131" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="E131" t="s" s="313">
         <v>215</v>
       </c>
-      <c r="F131" t="s">
+      <c r="F131" t="s" s="316">
         <v>215</v>
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="s" s="170">
+      <c r="A135" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B135" s="312"/>
+      <c r="C135" s="312"/>
+      <c r="D135" s="312"/>
+      <c r="E135" s="312"/>
+      <c r="F135" s="318"/>
     </row>
     <row r="136">
-      <c r="A136" t="s">
+      <c r="A136" t="s" s="314">
         <v>342</v>
       </c>
+      <c r="F136" s="315"/>
     </row>
     <row r="137">
-      <c r="A137" t="s">
+      <c r="A137" t="s" s="314">
         <v>343</v>
       </c>
+      <c r="F137" s="315"/>
     </row>
     <row r="138">
-      <c r="A138" t="s">
+      <c r="A138" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B138" t="s">
@@ -6532,12 +7132,12 @@
       <c r="E138" t="s">
         <v>269</v>
       </c>
-      <c r="F138" t="s">
+      <c r="F138" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="s">
+      <c r="A139" t="s" s="314">
         <v>5</v>
       </c>
       <c r="B139" t="s">
@@ -6552,47 +7152,54 @@
       <c r="E139" t="s">
         <v>193</v>
       </c>
-      <c r="F139" t="s">
+      <c r="F139" t="s" s="315">
         <v>216</v>
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="s">
+      <c r="A140" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C140" t="n">
+      <c r="C140" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" t="s" s="313">
         <v>216</v>
       </c>
-      <c r="E140" t="s">
-        <v>193</v>
-      </c>
-      <c r="F140" t="s">
+      <c r="E140" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="F140" t="s" s="316">
         <v>216</v>
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="s" s="171">
+      <c r="A144" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B144" s="312"/>
+      <c r="C144" s="312"/>
+      <c r="D144" s="312"/>
+      <c r="E144" s="312"/>
+      <c r="F144" s="318"/>
     </row>
     <row r="145">
-      <c r="A145" t="s">
+      <c r="A145" t="s" s="314">
         <v>344</v>
       </c>
+      <c r="F145" s="315"/>
     </row>
     <row r="146">
-      <c r="A146" t="s">
+      <c r="A146" t="s" s="314">
         <v>345</v>
       </c>
+      <c r="F146" s="315"/>
     </row>
     <row r="147">
-      <c r="A147" t="s">
+      <c r="A147" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B147" t="s">
@@ -6607,12 +7214,12 @@
       <c r="E147" t="s">
         <v>269</v>
       </c>
-      <c r="F147" t="s">
+      <c r="F147" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="s">
+      <c r="A148" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B148" t="s">
@@ -6627,47 +7234,54 @@
       <c r="E148" t="s">
         <v>217</v>
       </c>
-      <c r="F148" t="s">
+      <c r="F148" t="s" s="315">
         <v>346</v>
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="s">
+      <c r="A149" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C149" t="n">
+      <c r="C149" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D149" t="s">
-        <v>193</v>
-      </c>
-      <c r="E149" t="s">
+      <c r="D149" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="E149" t="s" s="313">
         <v>217</v>
       </c>
-      <c r="F149" t="s">
+      <c r="F149" t="s" s="316">
         <v>217</v>
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="s" s="172">
+      <c r="A153" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B153" s="312"/>
+      <c r="C153" s="312"/>
+      <c r="D153" s="312"/>
+      <c r="E153" s="312"/>
+      <c r="F153" s="318"/>
     </row>
     <row r="154">
-      <c r="A154" t="s">
+      <c r="A154" t="s" s="314">
         <v>347</v>
       </c>
+      <c r="F154" s="315"/>
     </row>
     <row r="155">
-      <c r="A155" t="s">
+      <c r="A155" t="s" s="314">
         <v>348</v>
       </c>
+      <c r="F155" s="315"/>
     </row>
     <row r="156">
-      <c r="A156" t="s">
+      <c r="A156" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B156" t="s">
@@ -6682,12 +7296,12 @@
       <c r="E156" t="s">
         <v>269</v>
       </c>
-      <c r="F156" t="s">
+      <c r="F156" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="s">
+      <c r="A157" t="s" s="314">
         <v>5</v>
       </c>
       <c r="B157" t="s">
@@ -6702,12 +7316,12 @@
       <c r="E157" t="s">
         <v>303</v>
       </c>
-      <c r="F157" t="s">
+      <c r="F157" t="s" s="315">
         <v>349</v>
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="s">
+      <c r="A158" t="s" s="314">
         <v>153</v>
       </c>
       <c r="B158" t="s">
@@ -6722,47 +7336,54 @@
       <c r="E158" t="s">
         <v>350</v>
       </c>
-      <c r="F158" t="s">
+      <c r="F158" t="s" s="315">
         <v>351</v>
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="s">
+      <c r="A159" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C159" t="n">
+      <c r="C159" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D159" t="s">
-        <v>193</v>
-      </c>
-      <c r="E159" t="s">
+      <c r="D159" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="E159" t="s" s="313">
         <v>218</v>
       </c>
-      <c r="F159" t="s">
+      <c r="F159" t="s" s="316">
         <v>218</v>
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="s" s="173">
+      <c r="A163" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B163" s="312"/>
+      <c r="C163" s="312"/>
+      <c r="D163" s="312"/>
+      <c r="E163" s="312"/>
+      <c r="F163" s="318"/>
     </row>
     <row r="164">
-      <c r="A164" t="s">
+      <c r="A164" t="s" s="314">
         <v>352</v>
       </c>
+      <c r="F164" s="315"/>
     </row>
     <row r="165">
-      <c r="A165" t="s">
+      <c r="A165" t="s" s="314">
         <v>353</v>
       </c>
+      <c r="F165" s="315"/>
     </row>
     <row r="166">
-      <c r="A166" t="s">
+      <c r="A166" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B166" t="s">
@@ -6777,12 +7398,12 @@
       <c r="E166" t="s">
         <v>269</v>
       </c>
-      <c r="F166" t="s">
+      <c r="F166" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="s">
+      <c r="A167" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B167" t="s">
@@ -6797,47 +7418,54 @@
       <c r="E167" t="s">
         <v>220</v>
       </c>
-      <c r="F167" t="s">
+      <c r="F167" t="s" s="315">
         <v>354</v>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="s">
+      <c r="A168" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C168" t="n">
+      <c r="C168" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D168" t="s">
-        <v>193</v>
-      </c>
-      <c r="E168" t="s">
+      <c r="D168" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="E168" t="s" s="313">
         <v>220</v>
       </c>
-      <c r="F168" t="s">
+      <c r="F168" t="s" s="316">
         <v>220</v>
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="s" s="174">
+      <c r="A172" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B172" s="312"/>
+      <c r="C172" s="312"/>
+      <c r="D172" s="312"/>
+      <c r="E172" s="312"/>
+      <c r="F172" s="318"/>
     </row>
     <row r="173">
-      <c r="A173" t="s">
+      <c r="A173" t="s" s="314">
         <v>355</v>
       </c>
+      <c r="F173" s="315"/>
     </row>
     <row r="174">
-      <c r="A174" t="s">
+      <c r="A174" t="s" s="314">
         <v>356</v>
       </c>
+      <c r="F174" s="315"/>
     </row>
     <row r="175">
-      <c r="A175" t="s">
+      <c r="A175" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B175" t="s">
@@ -6852,12 +7480,12 @@
       <c r="E175" t="s">
         <v>269</v>
       </c>
-      <c r="F175" t="s">
+      <c r="F175" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="s">
+      <c r="A176" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B176" t="s">
@@ -6872,47 +7500,54 @@
       <c r="E176" t="s">
         <v>222</v>
       </c>
-      <c r="F176" t="s">
+      <c r="F176" t="s" s="315">
         <v>357</v>
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="s">
+      <c r="A177" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C177" t="n">
+      <c r="C177" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D177" t="s">
-        <v>193</v>
-      </c>
-      <c r="E177" t="s">
+      <c r="D177" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="E177" t="s" s="313">
         <v>222</v>
       </c>
-      <c r="F177" t="s">
+      <c r="F177" t="s" s="316">
         <v>222</v>
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="s" s="175">
+      <c r="A181" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B181" s="312"/>
+      <c r="C181" s="312"/>
+      <c r="D181" s="312"/>
+      <c r="E181" s="312"/>
+      <c r="F181" s="318"/>
     </row>
     <row r="182">
-      <c r="A182" t="s">
+      <c r="A182" t="s" s="314">
         <v>358</v>
       </c>
+      <c r="F182" s="315"/>
     </row>
     <row r="183">
-      <c r="A183" t="s">
+      <c r="A183" t="s" s="314">
         <v>359</v>
       </c>
+      <c r="F183" s="315"/>
     </row>
     <row r="184">
-      <c r="A184" t="s">
+      <c r="A184" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B184" t="s">
@@ -6927,12 +7562,12 @@
       <c r="E184" t="s">
         <v>269</v>
       </c>
-      <c r="F184" t="s">
+      <c r="F184" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="185">
-      <c r="A185" t="s">
+      <c r="A185" t="s" s="314">
         <v>64</v>
       </c>
       <c r="B185" t="s">
@@ -6947,12 +7582,12 @@
       <c r="E185" t="s">
         <v>360</v>
       </c>
-      <c r="F185" t="s">
+      <c r="F185" t="s" s="315">
         <v>361</v>
       </c>
     </row>
     <row r="186">
-      <c r="A186" t="s">
+      <c r="A186" t="s" s="314">
         <v>113</v>
       </c>
       <c r="B186" t="s">
@@ -6967,12 +7602,12 @@
       <c r="E186" t="s">
         <v>277</v>
       </c>
-      <c r="F186" t="s">
+      <c r="F186" t="s" s="315">
         <v>362</v>
       </c>
     </row>
     <row r="187">
-      <c r="A187" t="s">
+      <c r="A187" t="s" s="314">
         <v>127</v>
       </c>
       <c r="B187" t="s">
@@ -6987,12 +7622,12 @@
       <c r="E187" t="s">
         <v>193</v>
       </c>
-      <c r="F187" t="s">
+      <c r="F187" t="s" s="315">
         <v>363</v>
       </c>
     </row>
     <row r="188">
-      <c r="A188" t="s">
+      <c r="A188" t="s" s="314">
         <v>161</v>
       </c>
       <c r="B188" t="s">
@@ -7007,12 +7642,12 @@
       <c r="E188" t="s">
         <v>364</v>
       </c>
-      <c r="F188" t="s">
+      <c r="F188" t="s" s="315">
         <v>365</v>
       </c>
     </row>
     <row r="189">
-      <c r="A189" t="s">
+      <c r="A189" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B189" t="s">
@@ -7027,47 +7662,54 @@
       <c r="E189" t="s">
         <v>193</v>
       </c>
-      <c r="F189" t="s">
+      <c r="F189" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="s">
+      <c r="A190" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C190" t="n">
+      <c r="C190" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" t="s" s="313">
         <v>223</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" t="s" s="313">
         <v>223</v>
       </c>
-      <c r="F190" t="s">
+      <c r="F190" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="194">
-      <c r="A194" t="s" s="176">
+      <c r="A194" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B194" s="312"/>
+      <c r="C194" s="312"/>
+      <c r="D194" s="312"/>
+      <c r="E194" s="312"/>
+      <c r="F194" s="318"/>
     </row>
     <row r="195">
-      <c r="A195" t="s">
+      <c r="A195" t="s" s="314">
         <v>367</v>
       </c>
+      <c r="F195" s="315"/>
     </row>
     <row r="196">
-      <c r="A196" t="s">
+      <c r="A196" t="s" s="314">
         <v>368</v>
       </c>
+      <c r="F196" s="315"/>
     </row>
     <row r="197">
-      <c r="A197" t="s">
+      <c r="A197" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B197" t="s">
@@ -7082,12 +7724,12 @@
       <c r="E197" t="s">
         <v>269</v>
       </c>
-      <c r="F197" t="s">
+      <c r="F197" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="198">
-      <c r="A198" t="s">
+      <c r="A198" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B198" t="s">
@@ -7102,47 +7744,54 @@
       <c r="E198" t="s">
         <v>225</v>
       </c>
-      <c r="F198" t="s">
+      <c r="F198" t="s" s="315">
         <v>369</v>
       </c>
     </row>
     <row r="199">
-      <c r="A199" t="s">
+      <c r="A199" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C199" t="n">
+      <c r="C199" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D199" t="s">
-        <v>193</v>
-      </c>
-      <c r="E199" t="s">
+      <c r="D199" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="E199" t="s" s="313">
         <v>225</v>
       </c>
-      <c r="F199" t="s">
+      <c r="F199" t="s" s="316">
         <v>225</v>
       </c>
     </row>
     <row r="203">
-      <c r="A203" t="s" s="177">
+      <c r="A203" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B203" s="312"/>
+      <c r="C203" s="312"/>
+      <c r="D203" s="312"/>
+      <c r="E203" s="312"/>
+      <c r="F203" s="318"/>
     </row>
     <row r="204">
-      <c r="A204" t="s">
+      <c r="A204" t="s" s="314">
         <v>370</v>
       </c>
+      <c r="F204" s="315"/>
     </row>
     <row r="205">
-      <c r="A205" t="s">
+      <c r="A205" t="s" s="314">
         <v>371</v>
       </c>
+      <c r="F205" s="315"/>
     </row>
     <row r="206">
-      <c r="A206" t="s">
+      <c r="A206" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B206" t="s">
@@ -7157,12 +7806,12 @@
       <c r="E206" t="s">
         <v>269</v>
       </c>
-      <c r="F206" t="s">
+      <c r="F206" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="207">
-      <c r="A207" t="s">
+      <c r="A207" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B207" t="s">
@@ -7177,47 +7826,54 @@
       <c r="E207" t="s">
         <v>227</v>
       </c>
-      <c r="F207" t="s">
+      <c r="F207" t="s" s="315">
         <v>372</v>
       </c>
     </row>
     <row r="208">
-      <c r="A208" t="s">
+      <c r="A208" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C208" t="n">
+      <c r="C208" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D208" t="s">
-        <v>193</v>
-      </c>
-      <c r="E208" t="s">
+      <c r="D208" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="E208" t="s" s="313">
         <v>227</v>
       </c>
-      <c r="F208" t="s">
+      <c r="F208" t="s" s="316">
         <v>227</v>
       </c>
     </row>
     <row r="212">
-      <c r="A212" t="s" s="178">
+      <c r="A212" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B212" s="312"/>
+      <c r="C212" s="312"/>
+      <c r="D212" s="312"/>
+      <c r="E212" s="312"/>
+      <c r="F212" s="318"/>
     </row>
     <row r="213">
-      <c r="A213" t="s">
+      <c r="A213" t="s" s="314">
         <v>373</v>
       </c>
+      <c r="F213" s="315"/>
     </row>
     <row r="214">
-      <c r="A214" t="s">
+      <c r="A214" t="s" s="314">
         <v>374</v>
       </c>
+      <c r="F214" s="315"/>
     </row>
     <row r="215">
-      <c r="A215" t="s">
+      <c r="A215" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B215" t="s">
@@ -7232,12 +7888,12 @@
       <c r="E215" t="s">
         <v>269</v>
       </c>
-      <c r="F215" t="s">
+      <c r="F215" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="216">
-      <c r="A216" t="s">
+      <c r="A216" t="s" s="314">
         <v>5</v>
       </c>
       <c r="B216" t="s">
@@ -7252,12 +7908,12 @@
       <c r="E216" t="s">
         <v>325</v>
       </c>
-      <c r="F216" t="s">
+      <c r="F216" t="s" s="315">
         <v>375</v>
       </c>
     </row>
     <row r="217">
-      <c r="A217" t="s">
+      <c r="A217" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B217" t="s">
@@ -7272,47 +7928,54 @@
       <c r="E217" t="s">
         <v>214</v>
       </c>
-      <c r="F217" t="s">
+      <c r="F217" t="s" s="315">
         <v>376</v>
       </c>
     </row>
     <row r="218">
-      <c r="A218" t="s">
+      <c r="A218" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B218" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C218" t="n">
+      <c r="C218" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D218" t="s">
-        <v>193</v>
-      </c>
-      <c r="E218" t="s">
+      <c r="D218" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="E218" t="s" s="313">
         <v>228</v>
       </c>
-      <c r="F218" t="s">
+      <c r="F218" t="s" s="316">
         <v>228</v>
       </c>
     </row>
     <row r="222">
-      <c r="A222" t="s" s="179">
+      <c r="A222" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B222" s="312"/>
+      <c r="C222" s="312"/>
+      <c r="D222" s="312"/>
+      <c r="E222" s="312"/>
+      <c r="F222" s="318"/>
     </row>
     <row r="223">
-      <c r="A223" t="s">
+      <c r="A223" t="s" s="314">
         <v>377</v>
       </c>
+      <c r="F223" s="315"/>
     </row>
     <row r="224">
-      <c r="A224" t="s">
+      <c r="A224" t="s" s="314">
         <v>378</v>
       </c>
+      <c r="F224" s="315"/>
     </row>
     <row r="225">
-      <c r="A225" t="s">
+      <c r="A225" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B225" t="s">
@@ -7327,12 +7990,12 @@
       <c r="E225" t="s">
         <v>269</v>
       </c>
-      <c r="F225" t="s">
+      <c r="F225" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="226">
-      <c r="A226" t="s">
+      <c r="A226" t="s" s="314">
         <v>5</v>
       </c>
       <c r="B226" t="s">
@@ -7347,47 +8010,54 @@
       <c r="E226" t="s">
         <v>229</v>
       </c>
-      <c r="F226" t="s">
+      <c r="F226" t="s" s="315">
         <v>379</v>
       </c>
     </row>
     <row r="227">
-      <c r="A227" t="s">
+      <c r="A227" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B227" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C227" t="n">
+      <c r="C227" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D227" t="s">
-        <v>193</v>
-      </c>
-      <c r="E227" t="s">
+      <c r="D227" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="E227" t="s" s="313">
         <v>229</v>
       </c>
-      <c r="F227" t="s">
+      <c r="F227" t="s" s="316">
         <v>229</v>
       </c>
     </row>
     <row r="231">
-      <c r="A231" t="s" s="180">
+      <c r="A231" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B231" s="312"/>
+      <c r="C231" s="312"/>
+      <c r="D231" s="312"/>
+      <c r="E231" s="312"/>
+      <c r="F231" s="318"/>
     </row>
     <row r="232">
-      <c r="A232" t="s">
+      <c r="A232" t="s" s="314">
         <v>380</v>
       </c>
+      <c r="F232" s="315"/>
     </row>
     <row r="233">
-      <c r="A233" t="s">
+      <c r="A233" t="s" s="314">
         <v>381</v>
       </c>
+      <c r="F233" s="315"/>
     </row>
     <row r="234">
-      <c r="A234" t="s">
+      <c r="A234" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B234" t="s">
@@ -7402,12 +8072,12 @@
       <c r="E234" t="s">
         <v>269</v>
       </c>
-      <c r="F234" t="s">
+      <c r="F234" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="235">
-      <c r="A235" t="s">
+      <c r="A235" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B235" t="s">
@@ -7422,47 +8092,54 @@
       <c r="E235" t="s">
         <v>231</v>
       </c>
-      <c r="F235" t="s">
+      <c r="F235" t="s" s="315">
         <v>382</v>
       </c>
     </row>
     <row r="236">
-      <c r="A236" t="s">
+      <c r="A236" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B236" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C236" t="n">
+      <c r="C236" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D236" t="s">
-        <v>193</v>
-      </c>
-      <c r="E236" t="s">
+      <c r="D236" t="s" s="313">
+        <v>193</v>
+      </c>
+      <c r="E236" t="s" s="313">
         <v>231</v>
       </c>
-      <c r="F236" t="s">
+      <c r="F236" t="s" s="316">
         <v>231</v>
       </c>
     </row>
     <row r="240">
-      <c r="A240" t="s" s="181">
+      <c r="A240" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B240" s="312"/>
+      <c r="C240" s="312"/>
+      <c r="D240" s="312"/>
+      <c r="E240" s="312"/>
+      <c r="F240" s="318"/>
     </row>
     <row r="241">
-      <c r="A241" t="s">
+      <c r="A241" t="s" s="314">
         <v>383</v>
       </c>
+      <c r="F241" s="315"/>
     </row>
     <row r="242">
-      <c r="A242" t="s">
+      <c r="A242" t="s" s="314">
         <v>384</v>
       </c>
+      <c r="F242" s="315"/>
     </row>
     <row r="243">
-      <c r="A243" t="s">
+      <c r="A243" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B243" t="s">
@@ -7477,12 +8154,12 @@
       <c r="E243" t="s">
         <v>269</v>
       </c>
-      <c r="F243" t="s">
+      <c r="F243" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="244">
-      <c r="A244" t="s">
+      <c r="A244" t="s" s="314">
         <v>64</v>
       </c>
       <c r="B244" t="s">
@@ -7497,12 +8174,12 @@
       <c r="E244" t="s">
         <v>385</v>
       </c>
-      <c r="F244" t="s">
+      <c r="F244" t="s" s="315">
         <v>386</v>
       </c>
     </row>
     <row r="245">
-      <c r="A245" t="s">
+      <c r="A245" t="s" s="314">
         <v>113</v>
       </c>
       <c r="B245" t="s">
@@ -7517,12 +8194,12 @@
       <c r="E245" t="s">
         <v>304</v>
       </c>
-      <c r="F245" t="s">
+      <c r="F245" t="s" s="315">
         <v>387</v>
       </c>
     </row>
     <row r="246">
-      <c r="A246" t="s">
+      <c r="A246" t="s" s="314">
         <v>127</v>
       </c>
       <c r="B246" t="s">
@@ -7537,12 +8214,12 @@
       <c r="E246" t="s">
         <v>193</v>
       </c>
-      <c r="F246" t="s">
+      <c r="F246" t="s" s="315">
         <v>388</v>
       </c>
     </row>
     <row r="247">
-      <c r="A247" t="s">
+      <c r="A247" t="s" s="314">
         <v>161</v>
       </c>
       <c r="B247" t="s">
@@ -7557,12 +8234,12 @@
       <c r="E247" t="s">
         <v>389</v>
       </c>
-      <c r="F247" t="s">
+      <c r="F247" t="s" s="315">
         <v>390</v>
       </c>
     </row>
     <row r="248">
-      <c r="A248" t="s">
+      <c r="A248" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B248" t="s">
@@ -7577,47 +8254,54 @@
       <c r="E248" t="s">
         <v>193</v>
       </c>
-      <c r="F248" t="s">
+      <c r="F248" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="249">
-      <c r="A249" t="s">
+      <c r="A249" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B249" t="s">
+      <c r="B249" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C249" t="n">
+      <c r="C249" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D249" t="s">
+      <c r="D249" t="s" s="313">
         <v>232</v>
       </c>
-      <c r="E249" t="s">
+      <c r="E249" t="s" s="313">
         <v>232</v>
       </c>
-      <c r="F249" t="s">
+      <c r="F249" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="253">
-      <c r="A253" t="s" s="182">
+      <c r="A253" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B253" s="312"/>
+      <c r="C253" s="312"/>
+      <c r="D253" s="312"/>
+      <c r="E253" s="312"/>
+      <c r="F253" s="318"/>
     </row>
     <row r="254">
-      <c r="A254" t="s">
+      <c r="A254" t="s" s="314">
         <v>391</v>
       </c>
+      <c r="F254" s="315"/>
     </row>
     <row r="255">
-      <c r="A255" t="s">
+      <c r="A255" t="s" s="314">
         <v>392</v>
       </c>
+      <c r="F255" s="315"/>
     </row>
     <row r="256">
-      <c r="A256" t="s">
+      <c r="A256" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B256" t="s">
@@ -7632,12 +8316,12 @@
       <c r="E256" t="s">
         <v>269</v>
       </c>
-      <c r="F256" t="s">
+      <c r="F256" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="257">
-      <c r="A257" t="s">
+      <c r="A257" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B257" t="s">
@@ -7652,12 +8336,12 @@
       <c r="E257" t="s">
         <v>193</v>
       </c>
-      <c r="F257" t="s">
+      <c r="F257" t="s" s="315">
         <v>234</v>
       </c>
     </row>
     <row r="258">
-      <c r="A258" t="s">
+      <c r="A258" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B258" t="s">
@@ -7672,47 +8356,54 @@
       <c r="E258" t="s">
         <v>234</v>
       </c>
-      <c r="F258" t="s">
+      <c r="F258" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="259">
-      <c r="A259" t="s">
+      <c r="A259" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B259" t="s">
+      <c r="B259" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C259" t="n">
+      <c r="C259" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D259" t="s">
+      <c r="D259" t="s" s="313">
         <v>234</v>
       </c>
-      <c r="E259" t="s">
+      <c r="E259" t="s" s="313">
         <v>234</v>
       </c>
-      <c r="F259" t="s">
+      <c r="F259" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="263">
-      <c r="A263" t="s" s="183">
+      <c r="A263" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B263" s="312"/>
+      <c r="C263" s="312"/>
+      <c r="D263" s="312"/>
+      <c r="E263" s="312"/>
+      <c r="F263" s="318"/>
     </row>
     <row r="264">
-      <c r="A264" t="s">
+      <c r="A264" t="s" s="314">
         <v>393</v>
       </c>
+      <c r="F264" s="315"/>
     </row>
     <row r="265">
-      <c r="A265" t="s">
+      <c r="A265" t="s" s="314">
         <v>394</v>
       </c>
+      <c r="F265" s="315"/>
     </row>
     <row r="266">
-      <c r="A266" t="s">
+      <c r="A266" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B266" t="s">
@@ -7727,12 +8418,12 @@
       <c r="E266" t="s">
         <v>269</v>
       </c>
-      <c r="F266" t="s">
+      <c r="F266" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="267">
-      <c r="A267" t="s">
+      <c r="A267" t="s" s="314">
         <v>89</v>
       </c>
       <c r="B267" t="s">
@@ -7747,12 +8438,12 @@
       <c r="E267" t="s">
         <v>193</v>
       </c>
-      <c r="F267" t="s">
+      <c r="F267" t="s" s="315">
         <v>235</v>
       </c>
     </row>
     <row r="268">
-      <c r="A268" t="s">
+      <c r="A268" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B268" t="s">
@@ -7767,47 +8458,54 @@
       <c r="E268" t="s">
         <v>235</v>
       </c>
-      <c r="F268" t="s">
+      <c r="F268" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="269">
-      <c r="A269" t="s">
+      <c r="A269" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B269" t="s">
+      <c r="B269" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C269" t="n">
+      <c r="C269" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D269" t="s">
+      <c r="D269" t="s" s="313">
         <v>235</v>
       </c>
-      <c r="E269" t="s">
+      <c r="E269" t="s" s="313">
         <v>235</v>
       </c>
-      <c r="F269" t="s">
+      <c r="F269" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="273">
-      <c r="A273" t="s" s="184">
+      <c r="A273" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B273" s="312"/>
+      <c r="C273" s="312"/>
+      <c r="D273" s="312"/>
+      <c r="E273" s="312"/>
+      <c r="F273" s="318"/>
     </row>
     <row r="274">
-      <c r="A274" t="s">
+      <c r="A274" t="s" s="314">
         <v>395</v>
       </c>
+      <c r="F274" s="315"/>
     </row>
     <row r="275">
-      <c r="A275" t="s">
+      <c r="A275" t="s" s="314">
         <v>396</v>
       </c>
+      <c r="F275" s="315"/>
     </row>
     <row r="276">
-      <c r="A276" t="s">
+      <c r="A276" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B276" t="s">
@@ -7822,12 +8520,12 @@
       <c r="E276" t="s">
         <v>269</v>
       </c>
-      <c r="F276" t="s">
+      <c r="F276" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="277">
-      <c r="A277" t="s">
+      <c r="A277" t="s" s="314">
         <v>127</v>
       </c>
       <c r="B277" t="s">
@@ -7842,12 +8540,12 @@
       <c r="E277" t="s">
         <v>193</v>
       </c>
-      <c r="F277" t="s">
+      <c r="F277" t="s" s="315">
         <v>210</v>
       </c>
     </row>
     <row r="278">
-      <c r="A278" t="s">
+      <c r="A278" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B278" t="s">
@@ -7862,47 +8560,54 @@
       <c r="E278" t="s">
         <v>210</v>
       </c>
-      <c r="F278" t="s">
+      <c r="F278" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="279">
-      <c r="A279" t="s">
+      <c r="A279" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B279" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C279" t="n">
+      <c r="C279" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D279" t="s">
+      <c r="D279" t="s" s="313">
         <v>210</v>
       </c>
-      <c r="E279" t="s">
+      <c r="E279" t="s" s="313">
         <v>210</v>
       </c>
-      <c r="F279" t="s">
+      <c r="F279" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="283">
-      <c r="A283" t="s" s="185">
+      <c r="A283" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B283" s="312"/>
+      <c r="C283" s="312"/>
+      <c r="D283" s="312"/>
+      <c r="E283" s="312"/>
+      <c r="F283" s="318"/>
     </row>
     <row r="284">
-      <c r="A284" t="s">
+      <c r="A284" t="s" s="314">
         <v>397</v>
       </c>
+      <c r="F284" s="315"/>
     </row>
     <row r="285">
-      <c r="A285" t="s">
+      <c r="A285" t="s" s="314">
         <v>398</v>
       </c>
+      <c r="F285" s="315"/>
     </row>
     <row r="286">
-      <c r="A286" t="s">
+      <c r="A286" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B286" t="s">
@@ -7917,12 +8622,12 @@
       <c r="E286" t="s">
         <v>269</v>
       </c>
-      <c r="F286" t="s">
+      <c r="F286" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="287">
-      <c r="A287" t="s">
+      <c r="A287" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B287" t="s">
@@ -7937,12 +8642,12 @@
       <c r="E287" t="s">
         <v>193</v>
       </c>
-      <c r="F287" t="s">
+      <c r="F287" t="s" s="315">
         <v>215</v>
       </c>
     </row>
     <row r="288">
-      <c r="A288" t="s">
+      <c r="A288" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B288" t="s">
@@ -7957,47 +8662,54 @@
       <c r="E288" t="s">
         <v>215</v>
       </c>
-      <c r="F288" t="s">
+      <c r="F288" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="289">
-      <c r="A289" t="s">
+      <c r="A289" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B289" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C289" t="n">
+      <c r="C289" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D289" t="s">
+      <c r="D289" t="s" s="313">
         <v>215</v>
       </c>
-      <c r="E289" t="s">
+      <c r="E289" t="s" s="313">
         <v>215</v>
       </c>
-      <c r="F289" t="s">
+      <c r="F289" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="293">
-      <c r="A293" t="s" s="186">
+      <c r="A293" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B293" s="312"/>
+      <c r="C293" s="312"/>
+      <c r="D293" s="312"/>
+      <c r="E293" s="312"/>
+      <c r="F293" s="318"/>
     </row>
     <row r="294">
-      <c r="A294" t="s">
+      <c r="A294" t="s" s="314">
         <v>399</v>
       </c>
+      <c r="F294" s="315"/>
     </row>
     <row r="295">
-      <c r="A295" t="s">
+      <c r="A295" t="s" s="314">
         <v>400</v>
       </c>
+      <c r="F295" s="315"/>
     </row>
     <row r="296">
-      <c r="A296" t="s">
+      <c r="A296" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B296" t="s">
@@ -8012,12 +8724,12 @@
       <c r="E296" t="s">
         <v>269</v>
       </c>
-      <c r="F296" t="s">
+      <c r="F296" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="297">
-      <c r="A297" t="s">
+      <c r="A297" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B297" t="s">
@@ -8032,12 +8744,12 @@
       <c r="E297" t="s">
         <v>193</v>
       </c>
-      <c r="F297" t="s">
+      <c r="F297" t="s" s="315">
         <v>217</v>
       </c>
     </row>
     <row r="298">
-      <c r="A298" t="s">
+      <c r="A298" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B298" t="s">
@@ -8052,47 +8764,54 @@
       <c r="E298" t="s">
         <v>217</v>
       </c>
-      <c r="F298" t="s">
+      <c r="F298" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="299">
-      <c r="A299" t="s">
+      <c r="A299" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B299" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C299" t="n">
+      <c r="C299" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D299" t="s">
+      <c r="D299" t="s" s="313">
         <v>217</v>
       </c>
-      <c r="E299" t="s">
+      <c r="E299" t="s" s="313">
         <v>217</v>
       </c>
-      <c r="F299" t="s">
+      <c r="F299" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="303">
-      <c r="A303" t="s" s="187">
+      <c r="A303" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B303" s="312"/>
+      <c r="C303" s="312"/>
+      <c r="D303" s="312"/>
+      <c r="E303" s="312"/>
+      <c r="F303" s="318"/>
     </row>
     <row r="304">
-      <c r="A304" t="s">
+      <c r="A304" t="s" s="314">
         <v>401</v>
       </c>
+      <c r="F304" s="315"/>
     </row>
     <row r="305">
-      <c r="A305" t="s">
+      <c r="A305" t="s" s="314">
         <v>402</v>
       </c>
+      <c r="F305" s="315"/>
     </row>
     <row r="306">
-      <c r="A306" t="s">
+      <c r="A306" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B306" t="s">
@@ -8107,12 +8826,12 @@
       <c r="E306" t="s">
         <v>269</v>
       </c>
-      <c r="F306" t="s">
+      <c r="F306" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="307">
-      <c r="A307" t="s">
+      <c r="A307" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B307" t="s">
@@ -8127,12 +8846,12 @@
       <c r="E307" t="s">
         <v>193</v>
       </c>
-      <c r="F307" t="s">
+      <c r="F307" t="s" s="315">
         <v>237</v>
       </c>
     </row>
     <row r="308">
-      <c r="A308" t="s">
+      <c r="A308" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B308" t="s">
@@ -8147,47 +8866,54 @@
       <c r="E308" t="s">
         <v>237</v>
       </c>
-      <c r="F308" t="s">
+      <c r="F308" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="309">
-      <c r="A309" t="s">
+      <c r="A309" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B309" t="s">
+      <c r="B309" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C309" t="n">
+      <c r="C309" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D309" t="s">
+      <c r="D309" t="s" s="313">
         <v>237</v>
       </c>
-      <c r="E309" t="s">
+      <c r="E309" t="s" s="313">
         <v>237</v>
       </c>
-      <c r="F309" t="s">
+      <c r="F309" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="313">
-      <c r="A313" t="s" s="188">
+      <c r="A313" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B313" s="312"/>
+      <c r="C313" s="312"/>
+      <c r="D313" s="312"/>
+      <c r="E313" s="312"/>
+      <c r="F313" s="318"/>
     </row>
     <row r="314">
-      <c r="A314" t="s">
+      <c r="A314" t="s" s="314">
         <v>403</v>
       </c>
+      <c r="F314" s="315"/>
     </row>
     <row r="315">
-      <c r="A315" t="s">
+      <c r="A315" t="s" s="314">
         <v>404</v>
       </c>
+      <c r="F315" s="315"/>
     </row>
     <row r="316">
-      <c r="A316" t="s">
+      <c r="A316" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B316" t="s">
@@ -8202,12 +8928,12 @@
       <c r="E316" t="s">
         <v>269</v>
       </c>
-      <c r="F316" t="s">
+      <c r="F316" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="317">
-      <c r="A317" t="s">
+      <c r="A317" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B317" t="s">
@@ -8222,12 +8948,12 @@
       <c r="E317" t="s">
         <v>193</v>
       </c>
-      <c r="F317" t="s">
+      <c r="F317" t="s" s="315">
         <v>239</v>
       </c>
     </row>
     <row r="318">
-      <c r="A318" t="s">
+      <c r="A318" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B318" t="s">
@@ -8242,47 +8968,54 @@
       <c r="E318" t="s">
         <v>239</v>
       </c>
-      <c r="F318" t="s">
+      <c r="F318" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="319">
-      <c r="A319" t="s">
+      <c r="A319" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B319" t="s">
+      <c r="B319" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C319" t="n">
+      <c r="C319" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D319" t="s">
+      <c r="D319" t="s" s="313">
         <v>239</v>
       </c>
-      <c r="E319" t="s">
+      <c r="E319" t="s" s="313">
         <v>239</v>
       </c>
-      <c r="F319" t="s">
+      <c r="F319" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="323">
-      <c r="A323" t="s" s="189">
+      <c r="A323" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B323" s="312"/>
+      <c r="C323" s="312"/>
+      <c r="D323" s="312"/>
+      <c r="E323" s="312"/>
+      <c r="F323" s="318"/>
     </row>
     <row r="324">
-      <c r="A324" t="s">
+      <c r="A324" t="s" s="314">
         <v>405</v>
       </c>
+      <c r="F324" s="315"/>
     </row>
     <row r="325">
-      <c r="A325" t="s">
+      <c r="A325" t="s" s="314">
         <v>406</v>
       </c>
+      <c r="F325" s="315"/>
     </row>
     <row r="326">
-      <c r="A326" t="s">
+      <c r="A326" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B326" t="s">
@@ -8297,12 +9030,12 @@
       <c r="E326" t="s">
         <v>269</v>
       </c>
-      <c r="F326" t="s">
+      <c r="F326" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="327">
-      <c r="A327" t="s">
+      <c r="A327" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B327" t="s">
@@ -8317,12 +9050,12 @@
       <c r="E327" t="s">
         <v>193</v>
       </c>
-      <c r="F327" t="s">
+      <c r="F327" t="s" s="315">
         <v>241</v>
       </c>
     </row>
     <row r="328">
-      <c r="A328" t="s">
+      <c r="A328" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B328" t="s">
@@ -8337,47 +9070,54 @@
       <c r="E328" t="s">
         <v>241</v>
       </c>
-      <c r="F328" t="s">
+      <c r="F328" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="329">
-      <c r="A329" t="s">
+      <c r="A329" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B329" t="s">
+      <c r="B329" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C329" t="n">
+      <c r="C329" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D329" t="s">
+      <c r="D329" t="s" s="313">
         <v>241</v>
       </c>
-      <c r="E329" t="s">
+      <c r="E329" t="s" s="313">
         <v>241</v>
       </c>
-      <c r="F329" t="s">
+      <c r="F329" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="333">
-      <c r="A333" t="s" s="190">
+      <c r="A333" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B333" s="312"/>
+      <c r="C333" s="312"/>
+      <c r="D333" s="312"/>
+      <c r="E333" s="312"/>
+      <c r="F333" s="318"/>
     </row>
     <row r="334">
-      <c r="A334" t="s">
+      <c r="A334" t="s" s="314">
         <v>407</v>
       </c>
+      <c r="F334" s="315"/>
     </row>
     <row r="335">
-      <c r="A335" t="s">
+      <c r="A335" t="s" s="314">
         <v>408</v>
       </c>
+      <c r="F335" s="315"/>
     </row>
     <row r="336">
-      <c r="A336" t="s">
+      <c r="A336" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B336" t="s">
@@ -8392,12 +9132,12 @@
       <c r="E336" t="s">
         <v>269</v>
       </c>
-      <c r="F336" t="s">
+      <c r="F336" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="337">
-      <c r="A337" t="s">
+      <c r="A337" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B337" t="s">
@@ -8412,12 +9152,12 @@
       <c r="E337" t="s">
         <v>193</v>
       </c>
-      <c r="F337" t="s">
+      <c r="F337" t="s" s="315">
         <v>222</v>
       </c>
     </row>
     <row r="338">
-      <c r="A338" t="s">
+      <c r="A338" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B338" t="s">
@@ -8432,47 +9172,54 @@
       <c r="E338" t="s">
         <v>222</v>
       </c>
-      <c r="F338" t="s">
+      <c r="F338" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="339">
-      <c r="A339" t="s">
+      <c r="A339" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B339" t="s">
+      <c r="B339" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C339" t="n">
+      <c r="C339" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D339" t="s">
+      <c r="D339" t="s" s="313">
         <v>222</v>
       </c>
-      <c r="E339" t="s">
+      <c r="E339" t="s" s="313">
         <v>222</v>
       </c>
-      <c r="F339" t="s">
+      <c r="F339" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="343">
-      <c r="A343" t="s" s="191">
+      <c r="A343" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B343" s="312"/>
+      <c r="C343" s="312"/>
+      <c r="D343" s="312"/>
+      <c r="E343" s="312"/>
+      <c r="F343" s="318"/>
     </row>
     <row r="344">
-      <c r="A344" t="s">
+      <c r="A344" t="s" s="314">
         <v>409</v>
       </c>
+      <c r="F344" s="315"/>
     </row>
     <row r="345">
-      <c r="A345" t="s">
+      <c r="A345" t="s" s="314">
         <v>410</v>
       </c>
+      <c r="F345" s="315"/>
     </row>
     <row r="346">
-      <c r="A346" t="s">
+      <c r="A346" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B346" t="s">
@@ -8487,12 +9234,12 @@
       <c r="E346" t="s">
         <v>269</v>
       </c>
-      <c r="F346" t="s">
+      <c r="F346" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="347">
-      <c r="A347" t="s">
+      <c r="A347" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B347" t="s">
@@ -8507,12 +9254,12 @@
       <c r="E347" t="s">
         <v>193</v>
       </c>
-      <c r="F347" t="s">
+      <c r="F347" t="s" s="315">
         <v>244</v>
       </c>
     </row>
     <row r="348">
-      <c r="A348" t="s">
+      <c r="A348" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B348" t="s">
@@ -8527,47 +9274,54 @@
       <c r="E348" t="s">
         <v>244</v>
       </c>
-      <c r="F348" t="s">
+      <c r="F348" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="349">
-      <c r="A349" t="s">
+      <c r="A349" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B349" t="s">
+      <c r="B349" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C349" t="n">
+      <c r="C349" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D349" t="s">
+      <c r="D349" t="s" s="313">
         <v>244</v>
       </c>
-      <c r="E349" t="s">
+      <c r="E349" t="s" s="313">
         <v>244</v>
       </c>
-      <c r="F349" t="s">
+      <c r="F349" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="353">
-      <c r="A353" t="s" s="192">
+      <c r="A353" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B353" s="312"/>
+      <c r="C353" s="312"/>
+      <c r="D353" s="312"/>
+      <c r="E353" s="312"/>
+      <c r="F353" s="318"/>
     </row>
     <row r="354">
-      <c r="A354" t="s">
+      <c r="A354" t="s" s="314">
         <v>411</v>
       </c>
+      <c r="F354" s="315"/>
     </row>
     <row r="355">
-      <c r="A355" t="s">
+      <c r="A355" t="s" s="314">
         <v>412</v>
       </c>
+      <c r="F355" s="315"/>
     </row>
     <row r="356">
-      <c r="A356" t="s">
+      <c r="A356" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B356" t="s">
@@ -8582,12 +9336,12 @@
       <c r="E356" t="s">
         <v>269</v>
       </c>
-      <c r="F356" t="s">
+      <c r="F356" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="357">
-      <c r="A357" t="s">
+      <c r="A357" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B357" t="s">
@@ -8602,12 +9356,12 @@
       <c r="E357" t="s">
         <v>193</v>
       </c>
-      <c r="F357" t="s">
+      <c r="F357" t="s" s="315">
         <v>246</v>
       </c>
     </row>
     <row r="358">
-      <c r="A358" t="s">
+      <c r="A358" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B358" t="s">
@@ -8622,47 +9376,54 @@
       <c r="E358" t="s">
         <v>246</v>
       </c>
-      <c r="F358" t="s">
+      <c r="F358" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="359">
-      <c r="A359" t="s">
+      <c r="A359" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B359" t="s">
+      <c r="B359" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C359" t="n">
+      <c r="C359" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D359" t="s">
+      <c r="D359" t="s" s="313">
         <v>246</v>
       </c>
-      <c r="E359" t="s">
+      <c r="E359" t="s" s="313">
         <v>246</v>
       </c>
-      <c r="F359" t="s">
+      <c r="F359" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="363">
-      <c r="A363" t="s" s="193">
+      <c r="A363" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B363" s="312"/>
+      <c r="C363" s="312"/>
+      <c r="D363" s="312"/>
+      <c r="E363" s="312"/>
+      <c r="F363" s="318"/>
     </row>
     <row r="364">
-      <c r="A364" t="s">
+      <c r="A364" t="s" s="314">
         <v>413</v>
       </c>
+      <c r="F364" s="315"/>
     </row>
     <row r="365">
-      <c r="A365" t="s">
+      <c r="A365" t="s" s="314">
         <v>414</v>
       </c>
+      <c r="F365" s="315"/>
     </row>
     <row r="366">
-      <c r="A366" t="s">
+      <c r="A366" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B366" t="s">
@@ -8677,12 +9438,12 @@
       <c r="E366" t="s">
         <v>269</v>
       </c>
-      <c r="F366" t="s">
+      <c r="F366" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="367">
-      <c r="A367" t="s">
+      <c r="A367" t="s" s="314">
         <v>101</v>
       </c>
       <c r="B367" t="s">
@@ -8697,12 +9458,12 @@
       <c r="E367" t="s">
         <v>193</v>
       </c>
-      <c r="F367" t="s">
+      <c r="F367" t="s" s="315">
         <v>194</v>
       </c>
     </row>
     <row r="368">
-      <c r="A368" t="s">
+      <c r="A368" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B368" t="s">
@@ -8717,47 +9478,54 @@
       <c r="E368" t="s">
         <v>194</v>
       </c>
-      <c r="F368" t="s">
+      <c r="F368" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="369">
-      <c r="A369" t="s">
+      <c r="A369" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B369" t="s">
+      <c r="B369" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C369" t="n">
+      <c r="C369" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D369" t="s">
+      <c r="D369" t="s" s="313">
         <v>194</v>
       </c>
-      <c r="E369" t="s">
+      <c r="E369" t="s" s="313">
         <v>194</v>
       </c>
-      <c r="F369" t="s">
+      <c r="F369" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="373">
-      <c r="A373" t="s" s="194">
+      <c r="A373" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B373" s="312"/>
+      <c r="C373" s="312"/>
+      <c r="D373" s="312"/>
+      <c r="E373" s="312"/>
+      <c r="F373" s="318"/>
     </row>
     <row r="374">
-      <c r="A374" t="s">
+      <c r="A374" t="s" s="314">
         <v>415</v>
       </c>
+      <c r="F374" s="315"/>
     </row>
     <row r="375">
-      <c r="A375" t="s">
+      <c r="A375" t="s" s="314">
         <v>416</v>
       </c>
+      <c r="F375" s="315"/>
     </row>
     <row r="376">
-      <c r="A376" t="s">
+      <c r="A376" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B376" t="s">
@@ -8772,12 +9540,12 @@
       <c r="E376" t="s">
         <v>269</v>
       </c>
-      <c r="F376" t="s">
+      <c r="F376" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="377">
-      <c r="A377" t="s">
+      <c r="A377" t="s" s="314">
         <v>127</v>
       </c>
       <c r="B377" t="s">
@@ -8792,12 +9560,12 @@
       <c r="E377" t="s">
         <v>193</v>
       </c>
-      <c r="F377" t="s">
+      <c r="F377" t="s" s="315">
         <v>249</v>
       </c>
     </row>
     <row r="378">
-      <c r="A378" t="s">
+      <c r="A378" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B378" t="s">
@@ -8812,47 +9580,54 @@
       <c r="E378" t="s">
         <v>249</v>
       </c>
-      <c r="F378" t="s">
+      <c r="F378" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="379">
-      <c r="A379" t="s">
+      <c r="A379" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B379" t="s">
+      <c r="B379" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C379" t="n">
+      <c r="C379" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D379" t="s">
+      <c r="D379" t="s" s="313">
         <v>249</v>
       </c>
-      <c r="E379" t="s">
+      <c r="E379" t="s" s="313">
         <v>249</v>
       </c>
-      <c r="F379" t="s">
+      <c r="F379" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="383">
-      <c r="A383" t="s" s="195">
+      <c r="A383" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B383" s="312"/>
+      <c r="C383" s="312"/>
+      <c r="D383" s="312"/>
+      <c r="E383" s="312"/>
+      <c r="F383" s="318"/>
     </row>
     <row r="384">
-      <c r="A384" t="s">
+      <c r="A384" t="s" s="314">
         <v>417</v>
       </c>
+      <c r="F384" s="315"/>
     </row>
     <row r="385">
-      <c r="A385" t="s">
+      <c r="A385" t="s" s="314">
         <v>418</v>
       </c>
+      <c r="F385" s="315"/>
     </row>
     <row r="386">
-      <c r="A386" t="s">
+      <c r="A386" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B386" t="s">
@@ -8867,12 +9642,12 @@
       <c r="E386" t="s">
         <v>269</v>
       </c>
-      <c r="F386" t="s">
+      <c r="F386" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="387">
-      <c r="A387" t="s">
+      <c r="A387" t="s" s="314">
         <v>158</v>
       </c>
       <c r="B387" t="s">
@@ -8887,12 +9662,12 @@
       <c r="E387" t="s">
         <v>193</v>
       </c>
-      <c r="F387" t="s">
+      <c r="F387" t="s" s="315">
         <v>210</v>
       </c>
     </row>
     <row r="388">
-      <c r="A388" t="s">
+      <c r="A388" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B388" t="s">
@@ -8907,47 +9682,54 @@
       <c r="E388" t="s">
         <v>210</v>
       </c>
-      <c r="F388" t="s">
+      <c r="F388" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="389">
-      <c r="A389" t="s">
+      <c r="A389" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B389" t="s">
+      <c r="B389" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C389" t="n">
+      <c r="C389" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D389" t="s">
+      <c r="D389" t="s" s="313">
         <v>210</v>
       </c>
-      <c r="E389" t="s">
+      <c r="E389" t="s" s="313">
         <v>210</v>
       </c>
-      <c r="F389" t="s">
+      <c r="F389" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="393">
-      <c r="A393" t="s" s="196">
+      <c r="A393" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B393" s="312"/>
+      <c r="C393" s="312"/>
+      <c r="D393" s="312"/>
+      <c r="E393" s="312"/>
+      <c r="F393" s="318"/>
     </row>
     <row r="394">
-      <c r="A394" t="s">
+      <c r="A394" t="s" s="314">
         <v>419</v>
       </c>
+      <c r="F394" s="315"/>
     </row>
     <row r="395">
-      <c r="A395" t="s">
+      <c r="A395" t="s" s="314">
         <v>420</v>
       </c>
+      <c r="F395" s="315"/>
     </row>
     <row r="396">
-      <c r="A396" t="s">
+      <c r="A396" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B396" t="s">
@@ -8962,12 +9744,12 @@
       <c r="E396" t="s">
         <v>269</v>
       </c>
-      <c r="F396" t="s">
+      <c r="F396" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="397">
-      <c r="A397" t="s">
+      <c r="A397" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B397" t="s">
@@ -8982,12 +9764,12 @@
       <c r="E397" t="s">
         <v>193</v>
       </c>
-      <c r="F397" t="s">
+      <c r="F397" t="s" s="315">
         <v>252</v>
       </c>
     </row>
     <row r="398">
-      <c r="A398" t="s">
+      <c r="A398" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B398" t="s">
@@ -9002,47 +9784,54 @@
       <c r="E398" t="s">
         <v>252</v>
       </c>
-      <c r="F398" t="s">
+      <c r="F398" t="s" s="315">
         <v>193</v>
       </c>
     </row>
     <row r="399">
-      <c r="A399" t="s">
+      <c r="A399" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B399" t="s">
+      <c r="B399" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C399" t="n">
+      <c r="C399" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D399" t="s">
+      <c r="D399" t="s" s="313">
         <v>252</v>
       </c>
-      <c r="E399" t="s">
+      <c r="E399" t="s" s="313">
         <v>252</v>
       </c>
-      <c r="F399" t="s">
+      <c r="F399" t="s" s="316">
         <v>193</v>
       </c>
     </row>
     <row r="403">
-      <c r="A403" t="s" s="197">
+      <c r="A403" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B403" s="312"/>
+      <c r="C403" s="312"/>
+      <c r="D403" s="312"/>
+      <c r="E403" s="312"/>
+      <c r="F403" s="318"/>
     </row>
     <row r="404">
-      <c r="A404" t="s">
+      <c r="A404" t="s" s="314">
         <v>421</v>
       </c>
+      <c r="F404" s="315"/>
     </row>
     <row r="405">
-      <c r="A405" t="s">
+      <c r="A405" t="s" s="314">
         <v>422</v>
       </c>
+      <c r="F405" s="315"/>
     </row>
     <row r="406">
-      <c r="A406" t="s">
+      <c r="A406" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B406" t="s">
@@ -9057,12 +9846,12 @@
       <c r="E406" t="s">
         <v>269</v>
       </c>
-      <c r="F406" t="s">
+      <c r="F406" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="407">
-      <c r="A407" t="s">
+      <c r="A407" t="s" s="314">
         <v>64</v>
       </c>
       <c r="B407" t="s">
@@ -9077,12 +9866,12 @@
       <c r="E407" t="s">
         <v>193</v>
       </c>
-      <c r="F407" t="s">
+      <c r="F407" t="s" s="315">
         <v>321</v>
       </c>
     </row>
     <row r="408">
-      <c r="A408" t="s">
+      <c r="A408" t="s" s="314">
         <v>113</v>
       </c>
       <c r="B408" t="s">
@@ -9097,12 +9886,12 @@
       <c r="E408" t="s">
         <v>193</v>
       </c>
-      <c r="F408" t="s">
+      <c r="F408" t="s" s="315">
         <v>423</v>
       </c>
     </row>
     <row r="409">
-      <c r="A409" t="s">
+      <c r="A409" t="s" s="314">
         <v>127</v>
       </c>
       <c r="B409" t="s">
@@ -9117,12 +9906,12 @@
       <c r="E409" t="s">
         <v>255</v>
       </c>
-      <c r="F409" t="s">
+      <c r="F409" t="s" s="315">
         <v>424</v>
       </c>
     </row>
     <row r="410">
-      <c r="A410" t="s">
+      <c r="A410" t="s" s="314">
         <v>161</v>
       </c>
       <c r="B410" t="s">
@@ -9137,12 +9926,12 @@
       <c r="E410" t="s">
         <v>193</v>
       </c>
-      <c r="F410" t="s">
+      <c r="F410" t="s" s="315">
         <v>256</v>
       </c>
     </row>
     <row r="411">
-      <c r="A411" t="s">
+      <c r="A411" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B411" t="s">
@@ -9157,47 +9946,54 @@
       <c r="E411" t="s">
         <v>425</v>
       </c>
-      <c r="F411" t="s">
+      <c r="F411" t="s" s="315">
         <v>426</v>
       </c>
     </row>
     <row r="412">
-      <c r="A412" t="s">
+      <c r="A412" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B412" t="s">
+      <c r="B412" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C412" t="n">
+      <c r="C412" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D412" t="s">
+      <c r="D412" t="s" s="313">
         <v>254</v>
       </c>
-      <c r="E412" t="s">
+      <c r="E412" t="s" s="313">
         <v>427</v>
       </c>
-      <c r="F412" t="s">
+      <c r="F412" t="s" s="316">
         <v>428</v>
       </c>
     </row>
     <row r="416">
-      <c r="A416" t="s" s="198">
+      <c r="A416" t="s" s="319">
         <v>262</v>
       </c>
+      <c r="B416" s="312"/>
+      <c r="C416" s="312"/>
+      <c r="D416" s="312"/>
+      <c r="E416" s="312"/>
+      <c r="F416" s="318"/>
     </row>
     <row r="417">
-      <c r="A417" t="s">
+      <c r="A417" t="s" s="314">
         <v>429</v>
       </c>
+      <c r="F417" s="315"/>
     </row>
     <row r="418">
-      <c r="A418" t="s">
+      <c r="A418" t="s" s="314">
         <v>430</v>
       </c>
+      <c r="F418" s="315"/>
     </row>
     <row r="419">
-      <c r="A419" t="s">
+      <c r="A419" t="s" s="314">
         <v>265</v>
       </c>
       <c r="B419" t="s">
@@ -9212,12 +10008,12 @@
       <c r="E419" t="s">
         <v>269</v>
       </c>
-      <c r="F419" t="s">
+      <c r="F419" t="s" s="315">
         <v>270</v>
       </c>
     </row>
     <row r="420">
-      <c r="A420" t="s">
+      <c r="A420" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B420" t="s">
@@ -9232,12 +10028,12 @@
       <c r="E420" t="s">
         <v>233</v>
       </c>
-      <c r="F420" t="s">
+      <c r="F420" t="s" s="315">
         <v>390</v>
       </c>
     </row>
     <row r="421">
-      <c r="A421" t="s">
+      <c r="A421" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B421" t="s">
@@ -9252,12 +10048,12 @@
       <c r="E421" t="s">
         <v>193</v>
       </c>
-      <c r="F421" t="s">
+      <c r="F421" t="s" s="315">
         <v>382</v>
       </c>
     </row>
     <row r="422">
-      <c r="A422" t="s">
+      <c r="A422" t="s" s="314">
         <v>169</v>
       </c>
       <c r="B422" t="s">
@@ -9272,27 +10068,27 @@
       <c r="E422" t="s">
         <v>193</v>
       </c>
-      <c r="F422" t="s">
+      <c r="F422" t="s" s="315">
         <v>432</v>
       </c>
     </row>
     <row r="423">
-      <c r="A423" t="s">
+      <c r="A423" t="s" s="317">
         <v>280</v>
       </c>
-      <c r="B423" t="s">
+      <c r="B423" t="s" s="313">
         <v>281</v>
       </c>
-      <c r="C423" t="n">
+      <c r="C423" t="n" s="313">
         <v>0.0</v>
       </c>
-      <c r="D423" t="s">
+      <c r="D423" t="s" s="313">
         <v>233</v>
       </c>
-      <c r="E423" t="s">
+      <c r="E423" t="s" s="313">
         <v>233</v>
       </c>
-      <c r="F423" t="s">
+      <c r="F423" t="s" s="316">
         <v>433</v>
       </c>
     </row>
@@ -9432,17 +10228,17 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="199">
+      <c r="A1" t="s" s="360">
         <v>434</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="200">
+      <c r="A2" t="s" s="361">
         <v>96</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="201">
+      <c r="A3" t="s" s="362">
         <v>435</v>
       </c>
     </row>
@@ -9700,17 +10496,17 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="202">
+      <c r="A1" t="s" s="363">
         <v>434</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="203">
+      <c r="A2" t="s" s="364">
         <v>96</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="204">
+      <c r="A3" t="s" s="365">
         <v>435</v>
       </c>
     </row>

</xml_diff>